<commit_message>
mag bug fixes, added min/max range finder settings
</commit_message>
<xml_diff>
--- a/AeroQuad_ICD.xlsx
+++ b/AeroQuad_ICD.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="226" uniqueCount="196">
   <si>
     <t>Commands</t>
   </si>
@@ -597,6 +597,12 @@
   </si>
   <si>
     <t>read vehicle state variable</t>
+  </si>
+  <si>
+    <t>range finder</t>
+  </si>
+  <si>
+    <t>read range finder</t>
   </si>
 </sst>
 </file>
@@ -1046,7 +1052,7 @@
   <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="H33" sqref="H33"/>
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1394,12 +1400,16 @@
       <c r="B23" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="4" t="s">
+        <v>194</v>
+      </c>
       <c r="D23" s="4"/>
       <c r="E23" s="3" t="s">
         <v>82</v>
       </c>
-      <c r="F23" s="4"/>
+      <c r="F23" s="4" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24" s="4"/>

</xml_diff>